<commit_message>
Release 8.00 'Friedrich Dürrenmatt'
</commit_message>
<xml_diff>
--- a/Images/Style_Function_table_style_professionally.xlsx
+++ b/Images/Style_Function_table_style_professionally.xlsx
@@ -353,7 +353,7 @@
     </fill>
   </fills>
   <!-- $Insert Borders$ -->
-  <borders count="7">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -362,91 +362,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="{'medium','#FF0000'}">
+      <left style="medium">
         <color rgb="FFFF0000"/>
       </left>
-      <right style="{'medium','#FF0000'}">
+      <right style="medium">
         <color rgb="FFFF0000"/>
       </right>
-      <top style="{'medium','#FF0000'}">
+      <top style="medium">
         <color rgb="FFFF0000"/>
       </top>
-      <bottom style="{'medium','#FF0000'}">
-        <color rgb="FFFF0000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="{'medium','#FF0000'}">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right style="{'medium','#FF0000'}">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top style="{'medium','#FF0000'}">
-        <color rgb="FFFF0000"/>
-      </top>
-      <bottom style="{'medium','#FF0000'}">
-        <color rgb="FFFF0000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="{'medium','#FF0000'}">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right style="{'medium','#FF0000'}">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top style="{'medium','#FF0000'}">
-        <color rgb="FFFF0000"/>
-      </top>
-      <bottom style="{'medium','#FF0000'}">
-        <color rgb="FFFF0000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="{'medium','#FF0000'}">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right style="{'medium','#FF0000'}">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top style="{'medium','#FF0000'}">
-        <color rgb="FFFF0000"/>
-      </top>
-      <bottom style="{'medium','#FF0000'}">
-        <color rgb="FFFF0000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="{'medium','#FF0000'}">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right style="{'medium','#FF0000'}">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top style="{'medium','#FF0000'}">
-        <color rgb="FFFF0000"/>
-      </top>
-      <bottom style="{'medium','#FF0000'}">
-        <color rgb="FFFF0000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="{'medium','#FF0000'}">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right style="{'medium','#FF0000'}">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top style="{'medium','#FF0000'}">
-        <color rgb="FFFF0000"/>
-      </top>
-      <bottom style="{'medium','#FF0000'}">
+      <bottom style="medium">
         <color rgb="FFFF0000"/>
       </bottom>
       <diagonal/>
@@ -456,7 +381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <!-- $Insert all Styles$ -->
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" borderId="0" fillId="0" fontId="0" xfId="0"/>
     <xf numFmtId="0" borderId="0" fillId="2" fontId="1" xfId="0" applyFill="1" applyFont="1">
       <alignment vertical="center" wrapText="1"/>
@@ -469,11 +394,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" borderId="1" fillId="4" fontId="4" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf numFmtId="0" borderId="2" fillId="4" fontId="5" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf numFmtId="0" borderId="3" fillId="4" fontId="4" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf numFmtId="0" borderId="4" fillId="4" fontId="5" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf numFmtId="0" borderId="5" fillId="4" fontId="4" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf numFmtId="0" borderId="6" fillId="4" fontId="5" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf numFmtId="0" borderId="1" fillId="4" fontId="5" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -993,7 +914,7 @@
       <c r="A8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C8" t="s">
@@ -1008,7 +929,7 @@
       <c r="F8" s="4">
         <v>24</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="6" t="s">
         <v>42</v>
       </c>
       <c r="H8" t="s">
@@ -1071,7 +992,7 @@
       <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C11"/>
@@ -1082,7 +1003,7 @@
         <v>56</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="6" t="s">
         <v>57</v>
       </c>
       <c r="H11" t="s">

</xml_diff>